<commit_message>
upload most recent data files
</commit_message>
<xml_diff>
--- a/data/Depression_Overview_Review_Data.xlsx
+++ b/data/Depression_Overview_Review_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon.sharepoint.com/sites/O365_HEDCOInstitute/Shared Documents/07 Research/01_Projects/01_Depression_Prevention_Overview/06_Report/02_Revision/01_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{A8996C0C-726C-4244-A260-85A11C68D76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FDBF9F-72D8-4ABC-9DF7-D7BE84E24C35}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{A8996C0C-726C-4244-A260-85A11C68D76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C62425A7-D104-4E0C-B645-808821E717CF}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{027D228C-667C-4781-8BE1-B447DEAFF92E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{027D228C-667C-4781-8BE1-B447DEAFF92E}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="499">
   <si>
     <t>Description</t>
   </si>
@@ -1654,6 +1654,9 @@
   </si>
   <si>
     <t>Two reviewers selected a sample of eligible studies and achieved good agreement (at least 80 percent) on a sample of representative studies, with the remainder selected by one reviewer.</t>
+  </si>
+  <si>
+    <t>Data were extracted by the first author only.</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5996A60D-0149-435A-A56C-E985C1B0A1D7}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BC1" sqref="BC1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
@@ -4342,10 +4345,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5656773-7495-4E4F-9F97-00C4E4E83822}">
   <dimension ref="A1:AK30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B187" sqref="B187"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="L6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.265625" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -4968,10 +4971,10 @@
         <v>406</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>395</v>
+        <v>498</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>164</v>
@@ -7238,17 +7241,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f91a1b-dc9e-4935-83bb-8b16b289603f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="031df1fd-70ca-41ea-9254-2ad0543794df" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8CAF755FF144545A9CBCE6353D30887" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bfe8ff3e518aeaf9cf3efde47ff8d751">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f91a1b-dc9e-4935-83bb-8b16b289603f" xmlns:ns3="031df1fd-70ca-41ea-9254-2ad0543794df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a636156854e892099ae02ea87682cd58" ns2:_="" ns3:_="">
     <xsd:import namespace="05f91a1b-dc9e-4935-83bb-8b16b289603f"/>
@@ -7485,6 +7477,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f91a1b-dc9e-4935-83bb-8b16b289603f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="031df1fd-70ca-41ea-9254-2ad0543794df" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD0BE5E-3032-47B6-8AA9-79A76644D852}">
   <ds:schemaRefs>
@@ -7494,17 +7497,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74BA74F3-FA5B-4D19-8DED-B1CBA6C516B8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="05f91a1b-dc9e-4935-83bb-8b16b289603f"/>
-    <ds:schemaRef ds:uri="031df1fd-70ca-41ea-9254-2ad0543794df"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0348837-C3EE-4CD9-BB65-1DE29E0AF56E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7521,4 +7513,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74BA74F3-FA5B-4D19-8DED-B1CBA6C516B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="05f91a1b-dc9e-4935-83bb-8b16b289603f"/>
+    <ds:schemaRef ds:uri="031df1fd-70ca-41ea-9254-2ad0543794df"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>